<commit_message>
Priya resolved place order issue
</commit_message>
<xml_diff>
--- a/Documents/AnasHandicraft/AHC Product List V1.xlsx
+++ b/Documents/AnasHandicraft/AHC Product List V1.xlsx
@@ -732,19 +732,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="20.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="21.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="23.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="45.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="1" width="8.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="23.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="15.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="16.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="13.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="23.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="15.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="23.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="15.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1014" min="29" style="1" width="8.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="1015" style="1" width="9.11"/>

</xml_diff>